<commit_message>
ENH: Primary implementation of ExcelRange
</commit_message>
<xml_diff>
--- a/modelx/tests/testdata/testdata.xlsx
+++ b/modelx/tests/testdata/testdata.xlsx
@@ -11,6 +11,9 @@
     <sheet name="TestSpaceTables" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="SampleTable">TestTables!$U$8:$Z$29</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -591,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AJ74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L71" sqref="L71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8:Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>

</xml_diff>